<commit_message>
changed seeds and email settings
</commit_message>
<xml_diff>
--- a/icons.xlsx
+++ b/icons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="480" windowWidth="23740" windowHeight="14180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>social_link_4</t>
   </si>
@@ -162,6 +162,105 @@
   </si>
   <si>
     <t>Top Icons</t>
+  </si>
+  <si>
+    <t>.fa-deviantart</t>
+  </si>
+  <si>
+    <t>.fa-digg</t>
+  </si>
+  <si>
+    <t>.fa-dribbble</t>
+  </si>
+  <si>
+    <t>.fa-etsy</t>
+  </si>
+  <si>
+    <t>.fa-facebook</t>
+  </si>
+  <si>
+    <t>.fa-flickr</t>
+  </si>
+  <si>
+    <t>.fa-foursquare</t>
+  </si>
+  <si>
+    <t>.fa-github</t>
+  </si>
+  <si>
+    <t>.fa-google-plus</t>
+  </si>
+  <si>
+    <t>.fa-houzz</t>
+  </si>
+  <si>
+    <t>.fa-instagram</t>
+  </si>
+  <si>
+    <t>.fa-linkedin</t>
+  </si>
+  <si>
+    <t>.fa-pinterest</t>
+  </si>
+  <si>
+    <t>.fa-quora</t>
+  </si>
+  <si>
+    <t>.fa-reddit</t>
+  </si>
+  <si>
+    <t>.fa-skype</t>
+  </si>
+  <si>
+    <t>.fa-slack</t>
+  </si>
+  <si>
+    <t>.fa-slideshare</t>
+  </si>
+  <si>
+    <t>.fa-snapchat</t>
+  </si>
+  <si>
+    <t>.fa-snapchat-ghost</t>
+  </si>
+  <si>
+    <t>.fa-soundcloud</t>
+  </si>
+  <si>
+    <t>.fa-spotify</t>
+  </si>
+  <si>
+    <t>.fa-stumbleupon</t>
+  </si>
+  <si>
+    <t>.fa-trello</t>
+  </si>
+  <si>
+    <t>.fa-tumblr</t>
+  </si>
+  <si>
+    <t>.fa-twitter</t>
+  </si>
+  <si>
+    <t>.fa-vimeo</t>
+  </si>
+  <si>
+    <t>.fa-vine</t>
+  </si>
+  <si>
+    <t>.fa-whatsapp</t>
+  </si>
+  <si>
+    <t>.fa-wikipedia-w</t>
+  </si>
+  <si>
+    <t>.fa-wordpress</t>
+  </si>
+  <si>
+    <t>.fa-yelp</t>
+  </si>
+  <si>
+    <t>.fa-youtube</t>
   </si>
 </sst>
 </file>
@@ -217,8 +316,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -244,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -255,6 +358,8 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -265,6 +370,8 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -858,10 +965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C7:L43"/>
+  <dimension ref="C6:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" workbookViewId="0">
-      <selection activeCell="L43" sqref="L11:L43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -869,25 +976,43 @@
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" customWidth="1"/>
-    <col min="9" max="9" width="29.1640625" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="29.1640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:12">
+    <row r="6" spans="3:20">
+      <c r="T6">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20">
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="3:12">
+      <c r="T7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20">
+      <c r="T8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20">
       <c r="H9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="3:12">
+      <c r="T9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="3:20">
       <c r="C11" t="s">
         <v>13</v>
       </c>
@@ -922,8 +1047,15 @@
         <f t="shared" ref="L11:L21" si="5">I11&amp;J11</f>
         <v>Icon.create!( :icon_css =&gt; "fa-deviantart", :name =&gt;"Deviantart", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="12" spans="3:12">
+      <c r="P11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T11">
+        <f>T6-T9-T8-T7</f>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20">
       <c r="C12" t="s">
         <v>14</v>
       </c>
@@ -932,8 +1064,8 @@
         <v>digg"</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
-        <v>"fa-digg"</v>
+        <f>""".fa-"&amp;D12</f>
+        <v>".fa-digg"</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -948,7 +1080,7 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" si="4"/>
-        <v>Icon.create!( :icon_css =&gt; "fa-digg"</v>
+        <v>Icon.create!( :icon_css =&gt; ".fa-digg"</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" ref="J12:J43" si="6">", :name =&gt;" &amp; G12 &amp;", :top_icons =&gt; " &amp; H12&amp;")"</f>
@@ -956,10 +1088,13 @@
       </c>
       <c r="L12" t="str">
         <f t="shared" si="5"/>
-        <v>Icon.create!( :icon_css =&gt; "fa-digg", :name =&gt;"Digg", :top_icons =&gt; FALSE)</v>
-      </c>
-    </row>
-    <row r="13" spans="3:12">
+        <v>Icon.create!( :icon_css =&gt; ".fa-digg", :name =&gt;"Digg", :top_icons =&gt; FALSE)</v>
+      </c>
+      <c r="P12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20">
       <c r="C13" t="s">
         <v>15</v>
       </c>
@@ -994,8 +1129,11 @@
         <f t="shared" si="5"/>
         <v>Icon.create!( :icon_css =&gt; "fa-dribbble", :name =&gt;"Dribbble", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="14" spans="3:12">
+      <c r="P13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="3:20">
       <c r="C14" t="s">
         <v>16</v>
       </c>
@@ -1030,8 +1168,11 @@
         <f t="shared" si="5"/>
         <v>Icon.create!( :icon_css =&gt; "fa-etsy", :name =&gt;"Etsy", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="15" spans="3:12">
+      <c r="P14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20">
       <c r="C15" t="s">
         <v>17</v>
       </c>
@@ -1066,8 +1207,11 @@
         <f t="shared" si="5"/>
         <v>Icon.create!( :icon_css =&gt; "fa-facebook", :name =&gt;"Facebook", :top_icons =&gt; TRUE)</v>
       </c>
-    </row>
-    <row r="16" spans="3:12">
+      <c r="P15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20">
       <c r="C16" t="s">
         <v>18</v>
       </c>
@@ -1102,8 +1246,11 @@
         <f t="shared" si="5"/>
         <v>Icon.create!( :icon_css =&gt; "fa-flickr", :name =&gt;"Flickr", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="17" spans="3:12">
+      <c r="P16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16">
       <c r="C17" t="s">
         <v>19</v>
       </c>
@@ -1138,8 +1285,11 @@
         <f t="shared" si="5"/>
         <v>Icon.create!( :icon_css =&gt; "fa-foursquare", :name =&gt;"Foursquare", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="18" spans="3:12">
+      <c r="P17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16">
       <c r="C18" t="s">
         <v>20</v>
       </c>
@@ -1174,8 +1324,11 @@
         <f t="shared" si="5"/>
         <v>Icon.create!( :icon_css =&gt; "fa-github", :name =&gt;"Github", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="19" spans="3:12">
+      <c r="P18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16">
       <c r="C19" t="s">
         <v>21</v>
       </c>
@@ -1210,8 +1363,11 @@
         <f t="shared" si="5"/>
         <v>Icon.create!( :icon_css =&gt; "fa-google-plus", :name =&gt;"Google-Plus", :top_icons =&gt; TRUE)</v>
       </c>
-    </row>
-    <row r="20" spans="3:12">
+      <c r="P19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16">
       <c r="C20" t="s">
         <v>22</v>
       </c>
@@ -1246,8 +1402,11 @@
         <f t="shared" si="5"/>
         <v>Icon.create!( :icon_css =&gt; "fa-houzz", :name =&gt;"Houzz", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="21" spans="3:12">
+      <c r="P20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16">
       <c r="C21" t="s">
         <v>23</v>
       </c>
@@ -1282,8 +1441,11 @@
         <f t="shared" si="5"/>
         <v>Icon.create!( :icon_css =&gt; "fa-instagram", :name =&gt;"Instagram", :top_icons =&gt; TRUE)</v>
       </c>
-    </row>
-    <row r="22" spans="3:12">
+      <c r="P21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16">
       <c r="C22" t="s">
         <v>24</v>
       </c>
@@ -1318,8 +1480,11 @@
         <f t="shared" ref="L22:L38" si="12">I22&amp;J22</f>
         <v>Icon.create!( :icon_css =&gt; "fa-linkedin", :name =&gt;"Linkedin", :top_icons =&gt; TRUE)</v>
       </c>
-    </row>
-    <row r="23" spans="3:12">
+      <c r="P22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16">
       <c r="C23" t="s">
         <v>25</v>
       </c>
@@ -1354,8 +1519,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-pinterest", :name =&gt;"Pinterest", :top_icons =&gt; TRUE)</v>
       </c>
-    </row>
-    <row r="24" spans="3:12">
+      <c r="P23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16">
       <c r="C24" t="s">
         <v>26</v>
       </c>
@@ -1390,8 +1558,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-quora", :name =&gt;"Quora", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="25" spans="3:12">
+      <c r="P24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="3:16">
       <c r="C25" t="s">
         <v>27</v>
       </c>
@@ -1426,8 +1597,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-reddit", :name =&gt;"Reddit", :top_icons =&gt; TRUE)</v>
       </c>
-    </row>
-    <row r="26" spans="3:12">
+      <c r="P25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="3:16">
       <c r="C26" t="s">
         <v>28</v>
       </c>
@@ -1462,8 +1636,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-skype", :name =&gt;"Skype", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="27" spans="3:12">
+      <c r="P26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="3:16">
       <c r="C27" t="s">
         <v>29</v>
       </c>
@@ -1498,8 +1675,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-slack", :name =&gt;"Slack", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="28" spans="3:12">
+      <c r="P27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16">
       <c r="C28" t="s">
         <v>30</v>
       </c>
@@ -1534,8 +1714,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-slideshare", :name =&gt;"Slideshare", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="29" spans="3:12">
+      <c r="P28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16">
       <c r="C29" t="s">
         <v>31</v>
       </c>
@@ -1570,8 +1753,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-snapchat", :name =&gt;"Snapchat", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="30" spans="3:12">
+      <c r="P29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="3:16">
       <c r="C30" t="s">
         <v>32</v>
       </c>
@@ -1606,8 +1792,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-snapchat-ghost", :name =&gt;"Snapchat-Ghost", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="31" spans="3:12">
+      <c r="P30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16">
       <c r="C31" t="s">
         <v>33</v>
       </c>
@@ -1642,8 +1831,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-soundcloud", :name =&gt;"Soundcloud", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="32" spans="3:12">
+      <c r="P31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16">
       <c r="C32" t="s">
         <v>34</v>
       </c>
@@ -1678,8 +1870,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-spotify", :name =&gt;"Spotify", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="33" spans="3:12">
+      <c r="P32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16">
       <c r="C33" t="s">
         <v>35</v>
       </c>
@@ -1714,8 +1909,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-stumbleupon", :name =&gt;"Stumbleupon", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="34" spans="3:12">
+      <c r="P33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="3:16">
       <c r="C34" t="s">
         <v>36</v>
       </c>
@@ -1750,8 +1948,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-trello", :name =&gt;"Trello", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="35" spans="3:12">
+      <c r="P34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16">
       <c r="C35" t="s">
         <v>37</v>
       </c>
@@ -1786,8 +1987,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-tumblr", :name =&gt;"Tumblr", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="36" spans="3:12">
+      <c r="P35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16">
       <c r="C36" t="s">
         <v>38</v>
       </c>
@@ -1822,8 +2026,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-twitter", :name =&gt;"Twitter", :top_icons =&gt; TRUE)</v>
       </c>
-    </row>
-    <row r="37" spans="3:12">
+      <c r="P36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="3:16">
       <c r="C37" t="s">
         <v>39</v>
       </c>
@@ -1858,8 +2065,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-vimeo", :name =&gt;"Vimeo", :top_icons =&gt; TRUE)</v>
       </c>
-    </row>
-    <row r="38" spans="3:12">
+      <c r="P37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="3:16">
       <c r="C38" t="s">
         <v>40</v>
       </c>
@@ -1894,8 +2104,11 @@
         <f t="shared" si="12"/>
         <v>Icon.create!( :icon_css =&gt; "fa-vine", :name =&gt;"Vine", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="39" spans="3:12">
+      <c r="P38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="3:16">
       <c r="C39" t="s">
         <v>41</v>
       </c>
@@ -1930,8 +2143,11 @@
         <f t="shared" ref="L39:L43" si="18">I39&amp;J39</f>
         <v>Icon.create!( :icon_css =&gt; "fa-whatsapp", :name =&gt;"Whatsapp", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="40" spans="3:12">
+      <c r="P39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="3:16">
       <c r="C40" t="s">
         <v>42</v>
       </c>
@@ -1966,8 +2182,11 @@
         <f t="shared" si="18"/>
         <v>Icon.create!( :icon_css =&gt; "fa-wikipedia-w", :name =&gt;"Wikipedia-W", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="41" spans="3:12">
+      <c r="P40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="3:16">
       <c r="C41" t="s">
         <v>43</v>
       </c>
@@ -2002,8 +2221,11 @@
         <f t="shared" si="18"/>
         <v>Icon.create!( :icon_css =&gt; "fa-wordpress", :name =&gt;"Wordpress", :top_icons =&gt; FALSE)</v>
       </c>
-    </row>
-    <row r="42" spans="3:12">
+      <c r="P41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="3:16">
       <c r="C42" t="s">
         <v>44</v>
       </c>
@@ -2038,8 +2260,11 @@
         <f t="shared" si="18"/>
         <v>Icon.create!( :icon_css =&gt; "fa-yelp", :name =&gt;"Yelp", :top_icons =&gt; TRUE)</v>
       </c>
-    </row>
-    <row r="43" spans="3:12">
+      <c r="P42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="3:16">
       <c r="C43" t="s">
         <v>45</v>
       </c>
@@ -2073,6 +2298,9 @@
       <c r="L43" t="str">
         <f t="shared" si="18"/>
         <v>Icon.create!( :icon_css =&gt; "fa-youtube", :name =&gt;"Youtube", :top_icons =&gt; TRUE)</v>
+      </c>
+      <c r="P43" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>